<commit_message>
Stationarity Test added for (State,Action) pair
</commit_message>
<xml_diff>
--- a/Brightkite_neew/p4-brightkite-0ms-annot.xlsx
+++ b/Brightkite_neew/p4-brightkite-0ms-annot.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\imMens Learning\Brightkite_neew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5A958A-6461-412A-965D-919EDAA04512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF91A80-F681-4492-80C7-12EA3929B5FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="144">
   <si>
     <t>proposition</t>
   </si>
@@ -519,6 +519,9 @@
   </si>
   <si>
     <t>2*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">so that means I’ll guess the startup is based in LA. </t>
   </si>
 </sst>
 </file>
@@ -1017,9 +1020,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1149,7 +1152,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>19</v>
@@ -1386,7 +1389,7 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>22</v>
@@ -1612,9 +1615,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>43</v>
+        <v>143</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
@@ -1646,7 +1649,7 @@
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>19</v>
@@ -1889,7 +1892,7 @@
         <v>0</v>
       </c>
       <c r="C33" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>14</v>
@@ -1915,7 +1918,7 @@
         <v>0</v>
       </c>
       <c r="C34" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>38</v>
@@ -2048,7 +2051,7 @@
         <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>18</v>
+        <v>112</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>11</v>
@@ -2100,7 +2103,7 @@
         <v>0</v>
       </c>
       <c r="C41" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>14</v>
@@ -2126,7 +2129,7 @@
         <v>0</v>
       </c>
       <c r="C42" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>14</v>
@@ -2528,7 +2531,7 @@
         <v>0</v>
       </c>
       <c r="C57" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>14</v>
@@ -2771,7 +2774,7 @@
         <v>0</v>
       </c>
       <c r="C66" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>44</v>
@@ -3008,7 +3011,7 @@
         <v>0</v>
       </c>
       <c r="C75" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
FAA dataset added and Q-Learning done with 2 state/action
</commit_message>
<xml_diff>
--- a/Brightkite_neew/p4-brightkite-0ms-annot.xlsx
+++ b/Brightkite_neew/p4-brightkite-0ms-annot.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\imMens Learning\Brightkite_neew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC315B2-6FD9-4165-9C51-8585A6FFE44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDAFEC4-6170-4DF0-B165-4A1084932C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7847,9 +7847,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06923B6-7230-4310-B02E-4FBA6A91B235}">
   <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
before adding new actions
</commit_message>
<xml_diff>
--- a/Brightkite_neew/p4-brightkite-0ms-annot.xlsx
+++ b/Brightkite_neew/p4-brightkite-0ms-annot.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\imMens Learning\Brightkite_neew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDAFEC4-6170-4DF0-B165-4A1084932C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751D2677-4EF4-4D03-A259-43DB50347857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1020,6 +1020,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:J87"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3354,7 +3357,7 @@
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup scale="24" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5693,7 +5696,7 @@
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6141,7 +6144,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7038,7 +7041,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7839,17 +7842,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06923B6-7230-4310-B02E-4FBA6A91B235}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:J87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10179,6 +10185,6 @@
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup scale="24" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>